<commit_message>
:card_file_box: updata datas from lab plot its graph
</commit_message>
<xml_diff>
--- a/5自动控制原理/1四旋翼飞行器建模实验/FrequentDomain.xlsx
+++ b/5自动控制原理/1四旋翼飞行器建模实验/FrequentDomain.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11720" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="13920" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="pitch" sheetId="1" r:id="rId1"/>
     <sheet name="yaw" sheetId="2" r:id="rId2"/>
+    <sheet name="param" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
   <si>
     <t>频率</t>
   </si>
@@ -25,16 +26,28 @@
   <si>
     <t>相位差</t>
   </si>
+  <si>
+    <t>外环控制器</t>
+  </si>
+  <si>
+    <t>内环控制器</t>
+  </si>
+  <si>
+    <t>俯仰pitch</t>
+  </si>
+  <si>
+    <t>偏航yaw</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -47,28 +60,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -82,6 +73,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -105,22 +111,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -134,57 +133,71 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -197,187 +210,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,8 +416,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.399975585192419"/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -412,8 +425,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.399975585192419"/>
       </bottom>
       <diagonal/>
     </border>
@@ -442,6 +455,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -453,21 +477,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -487,13 +496,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,154 +515,157 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1088,7 +1104,7 @@
   <sheetPr/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1198,4 +1214,83 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.4" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="1" spans="2:7">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>